<commit_message>
remove RT CASE PRICE
</commit_message>
<xml_diff>
--- a/UBP_Price.xlsx
+++ b/UBP_Price.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universalbeauty-my.sharepoint.com/personal/y_lee_universalbeauty_com/Documents/YoungSunLee/Develop/pricecheck/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="415" documentId="8_{2EA92289-AFF7-45F3-94D3-4549B2A8F483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4885C678-9C96-4C19-96CF-67E0C06ED6FF}"/>
+  <xr:revisionPtr revIDLastSave="417" documentId="8_{2EA92289-AFF7-45F3-94D3-4549B2A8F483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEFC9F38-AC29-4AF2-AF2B-7BC099FEEEB6}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{180F7D42-C005-46EA-91A1-F109AC7E0FF3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="490">
   <si>
     <t xml:space="preserve">ITEM NO. </t>
   </si>
@@ -1506,9 +1506,6 @@
   </si>
   <si>
     <t>RT UNIT PRICE</t>
-  </si>
-  <si>
-    <t>RT CASE PRICE</t>
   </si>
 </sst>
 </file>
@@ -1924,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73585EB-007D-4419-8C5C-3CFF5813C644}">
-  <dimension ref="A1:I242"/>
+  <dimension ref="A1:H242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,10 +1937,9 @@
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1968,11 +1964,8 @@
       <c r="H1" s="5" t="s">
         <v>489</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>29407</v>
       </c>
@@ -1997,11 +1990,8 @@
       <c r="H2">
         <v>4.34</v>
       </c>
-      <c r="I2">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>29420</v>
       </c>
@@ -2026,11 +2016,8 @@
       <c r="H3">
         <v>4.34</v>
       </c>
-      <c r="I3">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>29060</v>
       </c>
@@ -2055,11 +2042,8 @@
       <c r="H4">
         <v>4.34</v>
       </c>
-      <c r="I4">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>29066</v>
       </c>
@@ -2084,11 +2068,8 @@
       <c r="H5">
         <v>6.48</v>
       </c>
-      <c r="I5">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>29070</v>
       </c>
@@ -2113,11 +2094,8 @@
       <c r="H6">
         <v>4.34</v>
       </c>
-      <c r="I6">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>29076</v>
       </c>
@@ -2142,11 +2120,8 @@
       <c r="H7">
         <v>6.48</v>
       </c>
-      <c r="I7">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>29040</v>
       </c>
@@ -2171,11 +2146,8 @@
       <c r="H8">
         <v>4.34</v>
       </c>
-      <c r="I8">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>29042</v>
       </c>
@@ -2200,11 +2172,8 @@
       <c r="H9">
         <v>6.48</v>
       </c>
-      <c r="I9">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>29041</v>
       </c>
@@ -2229,11 +2198,8 @@
       <c r="H10">
         <v>4.34</v>
       </c>
-      <c r="I10">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>29043</v>
       </c>
@@ -2258,11 +2224,8 @@
       <c r="H11">
         <v>6.48</v>
       </c>
-      <c r="I11">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>29030</v>
       </c>
@@ -2287,11 +2250,8 @@
       <c r="H12">
         <v>4.34</v>
       </c>
-      <c r="I12">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>29300</v>
       </c>
@@ -2316,11 +2276,8 @@
       <c r="H13">
         <v>4.34</v>
       </c>
-      <c r="I13">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>29404</v>
       </c>
@@ -2345,11 +2302,8 @@
       <c r="H14">
         <v>4.34</v>
       </c>
-      <c r="I14">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>29406</v>
       </c>
@@ -2374,11 +2328,8 @@
       <c r="H15">
         <v>4.34</v>
       </c>
-      <c r="I15">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>29094</v>
       </c>
@@ -2403,11 +2354,8 @@
       <c r="H16">
         <v>4.34</v>
       </c>
-      <c r="I16">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>29020</v>
       </c>
@@ -2432,11 +2380,8 @@
       <c r="H17">
         <v>4.34</v>
       </c>
-      <c r="I17">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>29010</v>
       </c>
@@ -2461,11 +2406,8 @@
       <c r="H18">
         <v>6.48</v>
       </c>
-      <c r="I18">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>29093</v>
       </c>
@@ -2490,11 +2432,8 @@
       <c r="H19">
         <v>4.34</v>
       </c>
-      <c r="I19">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>29302</v>
       </c>
@@ -2519,11 +2458,8 @@
       <c r="H20">
         <v>6.48</v>
       </c>
-      <c r="I20">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>29050</v>
       </c>
@@ -2548,11 +2484,8 @@
       <c r="H21">
         <v>4.34</v>
       </c>
-      <c r="I21">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>29055</v>
       </c>
@@ -2577,11 +2510,8 @@
       <c r="H22">
         <v>6.48</v>
       </c>
-      <c r="I22">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>29080</v>
       </c>
@@ -2606,11 +2536,8 @@
       <c r="H23">
         <v>4.34</v>
       </c>
-      <c r="I23">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>29085</v>
       </c>
@@ -2635,11 +2562,8 @@
       <c r="H24">
         <v>6.48</v>
       </c>
-      <c r="I24">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>29401</v>
       </c>
@@ -2664,11 +2588,8 @@
       <c r="H25">
         <v>4.34</v>
       </c>
-      <c r="I25">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>29402</v>
       </c>
@@ -2693,11 +2614,8 @@
       <c r="H26">
         <v>6.48</v>
       </c>
-      <c r="I26">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>29405</v>
       </c>
@@ -2722,11 +2640,8 @@
       <c r="H27">
         <v>4.34</v>
       </c>
-      <c r="I27">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>29409</v>
       </c>
@@ -2751,11 +2666,8 @@
       <c r="H28">
         <v>6.48</v>
       </c>
-      <c r="I28">
-        <v>38.880000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>29092</v>
       </c>
@@ -2780,11 +2692,8 @@
       <c r="H29">
         <v>4.34</v>
       </c>
-      <c r="I29">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29304</v>
       </c>
@@ -2809,11 +2718,8 @@
       <c r="H30">
         <v>5.59</v>
       </c>
-      <c r="I30">
-        <v>33.54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>29095</v>
       </c>
@@ -2838,11 +2744,8 @@
       <c r="H31">
         <v>4.34</v>
       </c>
-      <c r="I31">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>29096</v>
       </c>
@@ -2867,11 +2770,8 @@
       <c r="H32">
         <v>4.34</v>
       </c>
-      <c r="I32">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29097</v>
       </c>
@@ -2896,11 +2796,8 @@
       <c r="H33">
         <v>4.34</v>
       </c>
-      <c r="I33">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>29098</v>
       </c>
@@ -2925,11 +2822,8 @@
       <c r="H34">
         <v>4.34</v>
       </c>
-      <c r="I34">
-        <v>26.04</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>2262</v>
       </c>
@@ -2954,11 +2848,8 @@
       <c r="H35">
         <v>5.33</v>
       </c>
-      <c r="I35">
-        <v>31.98</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>2263</v>
       </c>
@@ -2983,11 +2874,8 @@
       <c r="H36">
         <v>5.33</v>
       </c>
-      <c r="I36">
-        <v>31.98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2200</v>
       </c>
@@ -3012,11 +2900,8 @@
       <c r="H37">
         <v>3.36</v>
       </c>
-      <c r="I37">
-        <v>80.64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2202</v>
       </c>
@@ -3041,11 +2926,8 @@
       <c r="H38">
         <v>3.36</v>
       </c>
-      <c r="I38">
-        <v>80.64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>2201</v>
       </c>
@@ -3070,11 +2952,8 @@
       <c r="H39">
         <v>3.36</v>
       </c>
-      <c r="I39">
-        <v>80.64</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>2206</v>
       </c>
@@ -3099,11 +2978,8 @@
       <c r="H40">
         <v>3.36</v>
       </c>
-      <c r="I40">
-        <v>80.64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>2255</v>
       </c>
@@ -3128,11 +3004,8 @@
       <c r="H41">
         <v>5.71</v>
       </c>
-      <c r="I41">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>2256</v>
       </c>
@@ -3157,11 +3030,8 @@
       <c r="H42">
         <v>5.71</v>
       </c>
-      <c r="I42">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>2257</v>
       </c>
@@ -3186,11 +3056,8 @@
       <c r="H43">
         <v>5.71</v>
       </c>
-      <c r="I43">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>2258</v>
       </c>
@@ -3215,11 +3082,8 @@
       <c r="H44">
         <v>5.71</v>
       </c>
-      <c r="I44">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>2261</v>
       </c>
@@ -3244,11 +3108,8 @@
       <c r="H45">
         <v>5.71</v>
       </c>
-      <c r="I45">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>2265</v>
       </c>
@@ -3273,11 +3134,8 @@
       <c r="H46">
         <v>5.71</v>
       </c>
-      <c r="I46">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>2286</v>
       </c>
@@ -3302,11 +3160,8 @@
       <c r="H47">
         <v>5.71</v>
       </c>
-      <c r="I47">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>2287</v>
       </c>
@@ -3331,11 +3186,8 @@
       <c r="H48">
         <v>5.71</v>
       </c>
-      <c r="I48">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>2288</v>
       </c>
@@ -3360,11 +3212,8 @@
       <c r="H49">
         <v>5.71</v>
       </c>
-      <c r="I49">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>2289</v>
       </c>
@@ -3389,11 +3238,8 @@
       <c r="H50">
         <v>5.71</v>
       </c>
-      <c r="I50">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>2296</v>
       </c>
@@ -3418,11 +3264,8 @@
       <c r="H51">
         <v>5.71</v>
       </c>
-      <c r="I51">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>2295</v>
       </c>
@@ -3447,11 +3290,8 @@
       <c r="H52">
         <v>5.71</v>
       </c>
-      <c r="I52">
-        <v>34.26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>2316</v>
       </c>
@@ -3476,11 +3316,8 @@
       <c r="H53">
         <v>8.19</v>
       </c>
-      <c r="I53">
-        <v>49.14</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>2315</v>
       </c>
@@ -3505,11 +3342,8 @@
       <c r="H54">
         <v>8.19</v>
       </c>
-      <c r="I54">
-        <v>49.14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>2312</v>
       </c>
@@ -3534,11 +3368,8 @@
       <c r="H55">
         <v>8.19</v>
       </c>
-      <c r="I55">
-        <v>49.14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>81015</v>
       </c>
@@ -3563,11 +3394,8 @@
       <c r="H56">
         <v>5.39</v>
       </c>
-      <c r="I56">
-        <v>32.340000000000003</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>81016</v>
       </c>
@@ -3592,11 +3420,8 @@
       <c r="H57">
         <v>5.39</v>
       </c>
-      <c r="I57">
-        <v>32.340000000000003</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>81017</v>
       </c>
@@ -3621,11 +3446,8 @@
       <c r="H58">
         <v>5.39</v>
       </c>
-      <c r="I58">
-        <v>32.340000000000003</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>81018</v>
       </c>
@@ -3650,11 +3472,8 @@
       <c r="H59">
         <v>5.39</v>
       </c>
-      <c r="I59">
-        <v>32.340000000000003</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>81019</v>
       </c>
@@ -3679,11 +3498,8 @@
       <c r="H60">
         <v>5.39</v>
       </c>
-      <c r="I60">
-        <v>32.340000000000003</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>81022</v>
       </c>
@@ -3708,11 +3524,8 @@
       <c r="H61">
         <v>5.39</v>
       </c>
-      <c r="I61">
-        <v>32.340000000000003</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>81020</v>
       </c>
@@ -3731,11 +3544,8 @@
       <c r="H62">
         <v>107.8</v>
       </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>81921</v>
       </c>
@@ -3760,11 +3570,8 @@
       <c r="H63">
         <v>5.99</v>
       </c>
-      <c r="I63">
-        <v>35.94</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>81034</v>
       </c>
@@ -3789,11 +3596,8 @@
       <c r="H64">
         <v>8.99</v>
       </c>
-      <c r="I64">
-        <v>53.94</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>81976</v>
       </c>
@@ -3818,11 +3622,8 @@
       <c r="H65">
         <v>3.59</v>
       </c>
-      <c r="I65">
-        <v>43.08</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>81978</v>
       </c>
@@ -3847,11 +3648,8 @@
       <c r="H66">
         <v>5.39</v>
       </c>
-      <c r="I66">
-        <v>32.340000000000003</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>81024</v>
       </c>
@@ -3876,11 +3674,8 @@
       <c r="H67">
         <v>3.84</v>
       </c>
-      <c r="I67">
-        <v>23.04</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>76090</v>
       </c>
@@ -3905,11 +3700,8 @@
       <c r="H68">
         <v>6.95</v>
       </c>
-      <c r="I68">
-        <v>41.7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>76070</v>
       </c>
@@ -3934,11 +3726,8 @@
       <c r="H69">
         <v>6.95</v>
       </c>
-      <c r="I69">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>76086</v>
       </c>
@@ -3963,11 +3752,8 @@
       <c r="H70">
         <v>6.95</v>
       </c>
-      <c r="I70">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>76087</v>
       </c>
@@ -3992,11 +3778,8 @@
       <c r="H71">
         <v>6.95</v>
       </c>
-      <c r="I71">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>76083</v>
       </c>
@@ -4021,11 +3804,8 @@
       <c r="H72">
         <v>6.95</v>
       </c>
-      <c r="I72">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>76084</v>
       </c>
@@ -4050,11 +3830,8 @@
       <c r="H73">
         <v>6.95</v>
       </c>
-      <c r="I73">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>76085</v>
       </c>
@@ -4079,11 +3856,8 @@
       <c r="H74">
         <v>6.95</v>
       </c>
-      <c r="I74">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>76081</v>
       </c>
@@ -4108,11 +3882,8 @@
       <c r="H75">
         <v>6.95</v>
       </c>
-      <c r="I75">
-        <v>41.7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>81500</v>
       </c>
@@ -4137,11 +3908,8 @@
       <c r="H76">
         <v>6.95</v>
       </c>
-      <c r="I76">
-        <v>27.8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>76082</v>
       </c>
@@ -4166,11 +3934,8 @@
       <c r="H77">
         <v>6.95</v>
       </c>
-      <c r="I77">
-        <v>41.7</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>13059</v>
       </c>
@@ -4195,11 +3960,8 @@
       <c r="H78">
         <v>4.3099999999999996</v>
       </c>
-      <c r="I78">
-        <v>51.72</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>13061</v>
       </c>
@@ -4224,11 +3986,8 @@
       <c r="H79">
         <v>8.93</v>
       </c>
-      <c r="I79">
-        <v>53.58</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>13060</v>
       </c>
@@ -4253,11 +4012,8 @@
       <c r="H80">
         <v>4.3099999999999996</v>
       </c>
-      <c r="I80">
-        <v>51.72</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>13062</v>
       </c>
@@ -4282,11 +4038,8 @@
       <c r="H81">
         <v>8.93</v>
       </c>
-      <c r="I81">
-        <v>53.58</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81925</v>
       </c>
@@ -4311,11 +4064,8 @@
       <c r="H82">
         <v>1.79</v>
       </c>
-      <c r="I82">
-        <v>42.96</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>81926</v>
       </c>
@@ -4340,11 +4090,8 @@
       <c r="H83">
         <v>1.79</v>
       </c>
-      <c r="I83">
-        <v>42.96</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>81929</v>
       </c>
@@ -4369,11 +4116,8 @@
       <c r="H84">
         <v>1.79</v>
       </c>
-      <c r="I84">
-        <v>42.96</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>81932</v>
       </c>
@@ -4398,11 +4142,8 @@
       <c r="H85">
         <v>1.79</v>
       </c>
-      <c r="I85">
-        <v>42.96</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>81033</v>
       </c>
@@ -4427,11 +4168,8 @@
       <c r="H86">
         <v>1.79</v>
       </c>
-      <c r="I86">
-        <v>42.96</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>81927</v>
       </c>
@@ -4456,11 +4194,8 @@
       <c r="H87">
         <v>1.79</v>
       </c>
-      <c r="I87">
-        <v>42.96</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>81928</v>
       </c>
@@ -4485,11 +4220,8 @@
       <c r="H88">
         <v>1.79</v>
       </c>
-      <c r="I88">
-        <v>42.96</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>2001</v>
       </c>
@@ -4514,11 +4246,8 @@
       <c r="H89">
         <v>0.59</v>
       </c>
-      <c r="I89">
-        <v>84.96</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>2002</v>
       </c>
@@ -4543,11 +4272,8 @@
       <c r="H90">
         <v>1.21</v>
       </c>
-      <c r="I90">
-        <v>58.08</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>2003</v>
       </c>
@@ -4572,11 +4298,8 @@
       <c r="H91">
         <v>2.33</v>
       </c>
-      <c r="I91">
-        <v>55.92</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>2103</v>
       </c>
@@ -4601,11 +4324,8 @@
       <c r="H92">
         <v>0.76</v>
       </c>
-      <c r="I92">
-        <v>18.239999999999998</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>2441</v>
       </c>
@@ -4630,11 +4350,8 @@
       <c r="H93">
         <v>1.39</v>
       </c>
-      <c r="I93">
-        <v>16.68</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>2202</v>
       </c>
@@ -4659,11 +4376,8 @@
       <c r="H94">
         <v>0.66</v>
       </c>
-      <c r="I94">
-        <v>31.68</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>2204</v>
       </c>
@@ -4688,11 +4402,8 @@
       <c r="H95">
         <v>1.28</v>
       </c>
-      <c r="I95">
-        <v>61.44</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>2305</v>
       </c>
@@ -4717,11 +4428,8 @@
       <c r="H96">
         <v>1.68</v>
       </c>
-      <c r="I96">
-        <v>40.32</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>2306</v>
       </c>
@@ -4746,11 +4454,8 @@
       <c r="H97">
         <v>3.3</v>
       </c>
-      <c r="I97">
-        <v>39.6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>2416</v>
       </c>
@@ -4775,11 +4480,8 @@
       <c r="H98">
         <v>1.25</v>
       </c>
-      <c r="I98">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>2415</v>
       </c>
@@ -4804,11 +4506,8 @@
       <c r="H99">
         <v>2.4300000000000002</v>
       </c>
-      <c r="I99">
-        <v>58.32</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>2409</v>
       </c>
@@ -4833,11 +4532,8 @@
       <c r="H100">
         <v>4.49</v>
       </c>
-      <c r="I100">
-        <v>53.88</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>2448</v>
       </c>
@@ -4862,11 +4558,8 @@
       <c r="H101">
         <v>6.69</v>
       </c>
-      <c r="I101">
-        <v>80.28</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>2440</v>
       </c>
@@ -4891,11 +4584,8 @@
       <c r="H102">
         <v>2.9</v>
       </c>
-      <c r="I102">
-        <v>34.799999999999997</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>2404</v>
       </c>
@@ -4920,11 +4610,8 @@
       <c r="H103">
         <v>3.2</v>
       </c>
-      <c r="I103">
-        <v>76.8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>2408</v>
       </c>
@@ -4949,11 +4636,8 @@
       <c r="H104">
         <v>4.8099999999999996</v>
       </c>
-      <c r="I104">
-        <v>57.72</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>2414</v>
       </c>
@@ -4978,11 +4662,8 @@
       <c r="H105">
         <v>2.95</v>
       </c>
-      <c r="I105">
-        <v>35.4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>2410</v>
       </c>
@@ -5007,11 +4688,8 @@
       <c r="H106">
         <v>4.8099999999999996</v>
       </c>
-      <c r="I106">
-        <v>57.72</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>2411</v>
       </c>
@@ -5036,11 +4714,8 @@
       <c r="H107">
         <v>3.39</v>
       </c>
-      <c r="I107">
-        <v>40.68</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>2413</v>
       </c>
@@ -5065,11 +4740,8 @@
       <c r="H108">
         <v>1.87</v>
       </c>
-      <c r="I108">
-        <v>22.44</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>1012</v>
       </c>
@@ -5094,11 +4766,8 @@
       <c r="H109">
         <v>3.2</v>
       </c>
-      <c r="I109">
-        <v>38.4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>1204</v>
       </c>
@@ -5123,11 +4792,8 @@
       <c r="H110">
         <v>1.27</v>
       </c>
-      <c r="I110">
-        <v>15.24</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>1207</v>
       </c>
@@ -5152,11 +4818,8 @@
       <c r="H111">
         <v>2.2400000000000002</v>
       </c>
-      <c r="I111">
-        <v>26.88</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>1312</v>
       </c>
@@ -5181,11 +4844,8 @@
       <c r="H112">
         <v>3.4</v>
       </c>
-      <c r="I112">
-        <v>40.799999999999997</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>1404</v>
       </c>
@@ -5210,11 +4870,8 @@
       <c r="H113">
         <v>2.2400000000000002</v>
       </c>
-      <c r="I113">
-        <v>26.88</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>1412</v>
       </c>
@@ -5239,11 +4896,8 @@
       <c r="H114">
         <v>3.98</v>
       </c>
-      <c r="I114">
-        <v>47.76</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>2512</v>
       </c>
@@ -5268,11 +4922,8 @@
       <c r="H115">
         <v>3.52</v>
       </c>
-      <c r="I115">
-        <v>42.24</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>3304</v>
       </c>
@@ -5297,11 +4948,8 @@
       <c r="H116">
         <v>3.52</v>
       </c>
-      <c r="I116">
-        <v>42.24</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>3804</v>
       </c>
@@ -5326,11 +4974,8 @@
       <c r="H117" s="4">
         <v>3.29</v>
       </c>
-      <c r="I117" s="4">
-        <v>39.479999999999997</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>3404</v>
       </c>
@@ -5355,11 +5000,8 @@
       <c r="H118">
         <v>1.92</v>
       </c>
-      <c r="I118">
-        <v>23.04</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>3504</v>
       </c>
@@ -5384,11 +5026,8 @@
       <c r="H119">
         <v>1.92</v>
       </c>
-      <c r="I119">
-        <v>23.04</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
         <v>3904</v>
       </c>
@@ -5413,11 +5052,8 @@
       <c r="H120">
         <v>2.19</v>
       </c>
-      <c r="I120">
-        <v>26.28</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>3704</v>
       </c>
@@ -5442,11 +5078,8 @@
       <c r="H121" s="4">
         <v>2.19</v>
       </c>
-      <c r="I121" s="4">
-        <v>26.28</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>8109</v>
       </c>
@@ -5471,11 +5104,8 @@
       <c r="H122">
         <v>1.53</v>
       </c>
-      <c r="I122">
-        <v>18.36</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>6838</v>
       </c>
@@ -5500,11 +5130,8 @@
       <c r="H123">
         <v>3.4</v>
       </c>
-      <c r="I123">
-        <v>40.799999999999997</v>
-      </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>6839</v>
       </c>
@@ -5529,11 +5156,8 @@
       <c r="H124">
         <v>3.4</v>
       </c>
-      <c r="I124">
-        <v>40.799999999999997</v>
-      </c>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>8102</v>
       </c>
@@ -5558,11 +5182,8 @@
       <c r="H125">
         <v>1.64</v>
       </c>
-      <c r="I125">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>8103</v>
       </c>
@@ -5587,11 +5208,8 @@
       <c r="H126">
         <v>1.64</v>
       </c>
-      <c r="I126">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>8104</v>
       </c>
@@ -5616,11 +5234,8 @@
       <c r="H127">
         <v>1.64</v>
       </c>
-      <c r="I127">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>8105</v>
       </c>
@@ -5645,11 +5260,8 @@
       <c r="H128">
         <v>1.64</v>
       </c>
-      <c r="I128">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>8107</v>
       </c>
@@ -5671,11 +5283,8 @@
       <c r="H129">
         <v>78.67</v>
       </c>
-      <c r="I129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>8108</v>
       </c>
@@ -5700,11 +5309,8 @@
       <c r="H130">
         <v>1.64</v>
       </c>
-      <c r="I130">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>8111</v>
       </c>
@@ -5729,11 +5335,8 @@
       <c r="H131">
         <v>1.64</v>
       </c>
-      <c r="I131">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>8113</v>
       </c>
@@ -5758,11 +5361,8 @@
       <c r="H132">
         <v>1.64</v>
       </c>
-      <c r="I132">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>8114</v>
       </c>
@@ -5787,11 +5387,8 @@
       <c r="H133">
         <v>1.64</v>
       </c>
-      <c r="I133">
-        <v>19.68</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>8100</v>
       </c>
@@ -5813,11 +5410,8 @@
       <c r="H134">
         <v>78.67</v>
       </c>
-      <c r="I134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>2540</v>
       </c>
@@ -5842,11 +5436,8 @@
       <c r="H135">
         <v>4.49</v>
       </c>
-      <c r="I135">
-        <v>26.94</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>2621</v>
       </c>
@@ -5871,11 +5462,8 @@
       <c r="H136">
         <v>2.4300000000000002</v>
       </c>
-      <c r="I136">
-        <v>29.16</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>2620</v>
       </c>
@@ -5900,11 +5488,8 @@
       <c r="H137">
         <v>4.49</v>
       </c>
-      <c r="I137">
-        <v>53.88</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>2555</v>
       </c>
@@ -5929,11 +5514,8 @@
       <c r="H138">
         <v>12.84</v>
       </c>
-      <c r="I138">
-        <v>77.040000000000006</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>2556</v>
       </c>
@@ -5958,11 +5540,8 @@
       <c r="H139">
         <v>12.84</v>
       </c>
-      <c r="I139">
-        <v>77.040000000000006</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>2557</v>
       </c>
@@ -5987,11 +5566,8 @@
       <c r="H140">
         <v>6.41</v>
       </c>
-      <c r="I140">
-        <v>38.46</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>2558</v>
       </c>
@@ -6016,11 +5592,8 @@
       <c r="H141" s="4">
         <v>11.23</v>
       </c>
-      <c r="I141" s="4">
-        <v>67.38</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
         <v>8635</v>
       </c>
@@ -6045,11 +5618,8 @@
       <c r="H142">
         <v>3.84</v>
       </c>
-      <c r="I142">
-        <v>46.08</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>8636</v>
       </c>
@@ -6074,11 +5644,8 @@
       <c r="H143">
         <v>3.84</v>
       </c>
-      <c r="I143">
-        <v>46.08</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>8637</v>
       </c>
@@ -6103,11 +5670,8 @@
       <c r="H144">
         <v>6.99</v>
       </c>
-      <c r="I144">
-        <v>41.94</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>8638</v>
       </c>
@@ -6132,11 +5696,8 @@
       <c r="H145">
         <v>6.99</v>
       </c>
-      <c r="I145">
-        <v>41.94</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>807</v>
       </c>
@@ -6161,11 +5722,8 @@
       <c r="H146">
         <v>1.39</v>
       </c>
-      <c r="I146">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>808</v>
       </c>
@@ -6190,11 +5748,8 @@
       <c r="H147">
         <v>1.39</v>
       </c>
-      <c r="I147">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>809</v>
       </c>
@@ -6219,11 +5774,8 @@
       <c r="H148">
         <v>1.39</v>
       </c>
-      <c r="I148">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>810</v>
       </c>
@@ -6248,11 +5800,8 @@
       <c r="H149">
         <v>1.39</v>
       </c>
-      <c r="I149">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>811</v>
       </c>
@@ -6277,11 +5826,8 @@
       <c r="H150">
         <v>1.39</v>
       </c>
-      <c r="I150">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>826</v>
       </c>
@@ -6306,11 +5852,8 @@
       <c r="H151">
         <v>1.39</v>
       </c>
-      <c r="I151">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>813</v>
       </c>
@@ -6335,11 +5878,8 @@
       <c r="H152">
         <v>1.39</v>
       </c>
-      <c r="I152">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>814</v>
       </c>
@@ -6364,11 +5904,8 @@
       <c r="H153">
         <v>1.39</v>
       </c>
-      <c r="I153">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>816</v>
       </c>
@@ -6393,11 +5930,8 @@
       <c r="H154">
         <v>1.39</v>
       </c>
-      <c r="I154">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>817</v>
       </c>
@@ -6422,11 +5956,8 @@
       <c r="H155">
         <v>1.39</v>
       </c>
-      <c r="I155">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>821</v>
       </c>
@@ -6451,11 +5982,8 @@
       <c r="H156">
         <v>1.39</v>
       </c>
-      <c r="I156">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>822</v>
       </c>
@@ -6480,11 +6008,8 @@
       <c r="H157">
         <v>1.39</v>
       </c>
-      <c r="I157">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>823</v>
       </c>
@@ -6509,11 +6034,8 @@
       <c r="H158">
         <v>1.39</v>
       </c>
-      <c r="I158">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>824</v>
       </c>
@@ -6538,11 +6060,8 @@
       <c r="H159">
         <v>1.39</v>
       </c>
-      <c r="I159">
-        <v>8.34</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>907</v>
       </c>
@@ -6567,11 +6086,8 @@
       <c r="H160">
         <v>2.41</v>
       </c>
-      <c r="I160">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>909</v>
       </c>
@@ -6596,11 +6112,8 @@
       <c r="H161">
         <v>2.41</v>
       </c>
-      <c r="I161">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>911</v>
       </c>
@@ -6625,11 +6138,8 @@
       <c r="H162">
         <v>2.41</v>
       </c>
-      <c r="I162">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>926</v>
       </c>
@@ -6654,11 +6164,8 @@
       <c r="H163">
         <v>2.41</v>
       </c>
-      <c r="I163">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>916</v>
       </c>
@@ -6683,11 +6190,8 @@
       <c r="H164">
         <v>2.41</v>
       </c>
-      <c r="I164">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>921</v>
       </c>
@@ -6712,11 +6216,8 @@
       <c r="H165">
         <v>2.41</v>
       </c>
-      <c r="I165">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>923</v>
       </c>
@@ -6741,11 +6242,8 @@
       <c r="H166">
         <v>2.41</v>
       </c>
-      <c r="I166">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>924</v>
       </c>
@@ -6770,11 +6268,8 @@
       <c r="H167">
         <v>2.41</v>
       </c>
-      <c r="I167">
-        <v>14.46</v>
-      </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>57974</v>
       </c>
@@ -6799,11 +6294,8 @@
       <c r="H168">
         <v>0.75</v>
       </c>
-      <c r="I168">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>57975</v>
       </c>
@@ -6828,11 +6320,8 @@
       <c r="H169">
         <v>0.75</v>
       </c>
-      <c r="I169">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>57976</v>
       </c>
@@ -6857,11 +6346,8 @@
       <c r="H170">
         <v>0.75</v>
       </c>
-      <c r="I170">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
         <v>57977</v>
       </c>
@@ -6886,11 +6372,8 @@
       <c r="H171">
         <v>0.75</v>
       </c>
-      <c r="I171">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
         <v>57978</v>
       </c>
@@ -6915,11 +6398,8 @@
       <c r="H172">
         <v>0.75</v>
       </c>
-      <c r="I172">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
         <v>57979</v>
       </c>
@@ -6944,11 +6424,8 @@
       <c r="H173">
         <v>0.75</v>
       </c>
-      <c r="I173">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
         <v>57980</v>
       </c>
@@ -6973,11 +6450,8 @@
       <c r="H174">
         <v>0.75</v>
       </c>
-      <c r="I174">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
         <v>57981</v>
       </c>
@@ -7002,11 +6476,8 @@
       <c r="H175">
         <v>0.75</v>
       </c>
-      <c r="I175">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
         <v>57982</v>
       </c>
@@ -7031,11 +6502,8 @@
       <c r="H176">
         <v>0.75</v>
       </c>
-      <c r="I176">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
         <v>57983</v>
       </c>
@@ -7060,11 +6528,8 @@
       <c r="H177">
         <v>0.75</v>
       </c>
-      <c r="I177">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
         <v>57984</v>
       </c>
@@ -7089,11 +6554,8 @@
       <c r="H178">
         <v>0.75</v>
       </c>
-      <c r="I178">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
         <v>57985</v>
       </c>
@@ -7118,11 +6580,8 @@
       <c r="H179">
         <v>0.75</v>
       </c>
-      <c r="I179">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
         <v>57986</v>
       </c>
@@ -7147,11 +6606,8 @@
       <c r="H180">
         <v>0.75</v>
       </c>
-      <c r="I180">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
         <v>57987</v>
       </c>
@@ -7176,11 +6632,8 @@
       <c r="H181">
         <v>0.75</v>
       </c>
-      <c r="I181">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
         <v>57988</v>
       </c>
@@ -7205,11 +6658,8 @@
       <c r="H182">
         <v>0.75</v>
       </c>
-      <c r="I182">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
         <v>57989</v>
       </c>
@@ -7234,11 +6684,8 @@
       <c r="H183">
         <v>0.75</v>
       </c>
-      <c r="I183">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
         <v>57990</v>
       </c>
@@ -7263,11 +6710,8 @@
       <c r="H184">
         <v>0.75</v>
       </c>
-      <c r="I184">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
         <v>57991</v>
       </c>
@@ -7292,11 +6736,8 @@
       <c r="H185">
         <v>0.75</v>
       </c>
-      <c r="I185">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
         <v>58000</v>
       </c>
@@ -7321,11 +6762,8 @@
       <c r="H186">
         <v>0.75</v>
       </c>
-      <c r="I186">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
         <v>58001</v>
       </c>
@@ -7350,11 +6788,8 @@
       <c r="H187">
         <v>2.12</v>
       </c>
-      <c r="I187">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
         <v>58002</v>
       </c>
@@ -7379,11 +6814,8 @@
       <c r="H188">
         <v>2.12</v>
       </c>
-      <c r="I188">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
         <v>58003</v>
       </c>
@@ -7408,11 +6840,8 @@
       <c r="H189">
         <v>2.12</v>
       </c>
-      <c r="I189">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
         <v>58004</v>
       </c>
@@ -7437,11 +6866,8 @@
       <c r="H190">
         <v>2.12</v>
       </c>
-      <c r="I190">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
         <v>58005</v>
       </c>
@@ -7466,11 +6892,8 @@
       <c r="H191">
         <v>2.12</v>
       </c>
-      <c r="I191">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
         <v>58006</v>
       </c>
@@ -7495,11 +6918,8 @@
       <c r="H192">
         <v>2.12</v>
       </c>
-      <c r="I192">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
         <v>58007</v>
       </c>
@@ -7524,11 +6944,8 @@
       <c r="H193">
         <v>2.12</v>
       </c>
-      <c r="I193">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
         <v>58008</v>
       </c>
@@ -7553,11 +6970,8 @@
       <c r="H194">
         <v>2.12</v>
       </c>
-      <c r="I194">
-        <v>25.44</v>
-      </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
         <v>81872</v>
       </c>
@@ -7582,11 +6996,8 @@
       <c r="H195">
         <v>3.59</v>
       </c>
-      <c r="I195">
-        <v>21.54</v>
-      </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
         <v>81873</v>
       </c>
@@ -7611,11 +7022,8 @@
       <c r="H196">
         <v>3.59</v>
       </c>
-      <c r="I196">
-        <v>21.54</v>
-      </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
         <v>81874</v>
       </c>
@@ -7640,11 +7048,8 @@
       <c r="H197">
         <v>3.59</v>
       </c>
-      <c r="I197">
-        <v>21.54</v>
-      </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
         <v>81875</v>
       </c>
@@ -7669,11 +7074,8 @@
       <c r="H198">
         <v>3.59</v>
       </c>
-      <c r="I198">
-        <v>21.54</v>
-      </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
         <v>81876</v>
       </c>
@@ -7698,11 +7100,8 @@
       <c r="H199">
         <v>3.59</v>
       </c>
-      <c r="I199">
-        <v>21.54</v>
-      </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
         <v>81877</v>
       </c>
@@ -7727,11 +7126,8 @@
       <c r="H200">
         <v>3.59</v>
       </c>
-      <c r="I200">
-        <v>21.54</v>
-      </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
         <v>81916</v>
       </c>
@@ -7750,11 +7146,8 @@
       <c r="H201">
         <v>65</v>
       </c>
-      <c r="I201">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
         <v>8351</v>
       </c>
@@ -7779,11 +7172,8 @@
       <c r="H202">
         <v>4.3099999999999996</v>
       </c>
-      <c r="I202">
-        <v>51.72</v>
-      </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="2">
         <v>8352</v>
       </c>
@@ -7808,11 +7198,8 @@
       <c r="H203">
         <v>2.7</v>
       </c>
-      <c r="I203">
-        <v>32.4</v>
-      </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="2">
         <v>8353</v>
       </c>
@@ -7837,11 +7224,8 @@
       <c r="H204">
         <v>1.37</v>
       </c>
-      <c r="I204">
-        <v>32.880000000000003</v>
-      </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="2">
         <v>1904</v>
       </c>
@@ -7866,11 +7250,8 @@
       <c r="H205">
         <v>4.79</v>
       </c>
-      <c r="I205">
-        <v>28.74</v>
-      </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="2">
         <v>1901</v>
       </c>
@@ -7895,11 +7276,8 @@
       <c r="H206">
         <v>4.79</v>
       </c>
-      <c r="I206">
-        <v>28.74</v>
-      </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2">
         <v>1900</v>
       </c>
@@ -7924,11 +7302,8 @@
       <c r="H207">
         <v>4.79</v>
       </c>
-      <c r="I207">
-        <v>28.74</v>
-      </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="2">
         <v>1899</v>
       </c>
@@ -7953,11 +7328,8 @@
       <c r="H208">
         <v>4.79</v>
       </c>
-      <c r="I208">
-        <v>28.74</v>
-      </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="2">
         <v>1902</v>
       </c>
@@ -7982,11 +7354,8 @@
       <c r="H209">
         <v>4.79</v>
       </c>
-      <c r="I209">
-        <v>28.74</v>
-      </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
         <v>1903</v>
       </c>
@@ -8011,11 +7380,8 @@
       <c r="H210">
         <v>4.79</v>
       </c>
-      <c r="I210">
-        <v>28.74</v>
-      </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="2">
         <v>1905</v>
       </c>
@@ -8037,11 +7403,8 @@
       <c r="H211">
         <v>110.96</v>
       </c>
-      <c r="I211">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="2">
         <v>8390</v>
       </c>
@@ -8066,11 +7429,8 @@
       <c r="H212">
         <v>4.1900000000000004</v>
       </c>
-      <c r="I212">
-        <v>25.14</v>
-      </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="2">
         <v>8392</v>
       </c>
@@ -8095,11 +7455,8 @@
       <c r="H213">
         <v>4.1900000000000004</v>
       </c>
-      <c r="I213">
-        <v>25.14</v>
-      </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="2">
         <v>8393</v>
       </c>
@@ -8124,11 +7481,8 @@
       <c r="H214">
         <v>8.89</v>
       </c>
-      <c r="I214">
-        <v>53.34</v>
-      </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="2">
         <v>8394</v>
       </c>
@@ -8153,11 +7507,8 @@
       <c r="H215">
         <v>8.89</v>
       </c>
-      <c r="I215">
-        <v>53.34</v>
-      </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="2">
         <v>8380</v>
       </c>
@@ -8182,11 +7533,8 @@
       <c r="H216">
         <v>1.28</v>
       </c>
-      <c r="I216">
-        <v>7.68</v>
-      </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="2">
         <v>8384</v>
       </c>
@@ -8211,11 +7559,8 @@
       <c r="H217">
         <v>1.28</v>
       </c>
-      <c r="I217">
-        <v>7.68</v>
-      </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
         <v>8385</v>
       </c>
@@ -8240,11 +7585,8 @@
       <c r="H218">
         <v>2.11</v>
       </c>
-      <c r="I218">
-        <v>12.66</v>
-      </c>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="2">
         <v>8389</v>
       </c>
@@ -8269,11 +7611,8 @@
       <c r="H219">
         <v>2.11</v>
       </c>
-      <c r="I219">
-        <v>12.66</v>
-      </c>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="2">
         <v>81917</v>
       </c>
@@ -8298,11 +7637,8 @@
       <c r="H220">
         <v>1.5</v>
       </c>
-      <c r="I220">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="2">
         <v>81918</v>
       </c>
@@ -8327,11 +7663,8 @@
       <c r="H221">
         <v>2.5</v>
       </c>
-      <c r="I221">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="2">
         <v>81919</v>
       </c>
@@ -8356,11 +7689,8 @@
       <c r="H222">
         <v>1.5</v>
       </c>
-      <c r="I222">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="2">
         <v>81920</v>
       </c>
@@ -8385,11 +7715,8 @@
       <c r="H223">
         <v>2.5</v>
       </c>
-      <c r="I223">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2">
         <v>81861</v>
       </c>
@@ -8414,11 +7741,8 @@
       <c r="H224">
         <v>1.65</v>
       </c>
-      <c r="I224">
-        <v>118.8</v>
-      </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="2">
         <v>81862</v>
       </c>
@@ -8443,11 +7767,8 @@
       <c r="H225">
         <v>1.65</v>
       </c>
-      <c r="I225">
-        <v>118.8</v>
-      </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>81863</v>
       </c>
@@ -8472,11 +7793,8 @@
       <c r="H226">
         <v>3.25</v>
       </c>
-      <c r="I226">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="2">
         <v>81864</v>
       </c>
@@ -8501,11 +7819,8 @@
       <c r="H227">
         <v>3.25</v>
       </c>
-      <c r="I227">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="2">
         <v>24683</v>
       </c>
@@ -8530,11 +7845,8 @@
       <c r="H228">
         <v>1.19</v>
       </c>
-      <c r="I228">
-        <v>42.84</v>
-      </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A229" s="2">
         <v>24693</v>
       </c>
@@ -8559,11 +7871,8 @@
       <c r="H229">
         <v>1.19</v>
       </c>
-      <c r="I229">
-        <v>42.84</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A230" s="2">
         <v>411</v>
       </c>
@@ -8588,11 +7897,8 @@
       <c r="H230">
         <v>6.29</v>
       </c>
-      <c r="I230">
-        <v>37.74</v>
-      </c>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A231" s="2">
         <v>412</v>
       </c>
@@ -8617,11 +7923,8 @@
       <c r="H231">
         <v>6.29</v>
       </c>
-      <c r="I231">
-        <v>37.74</v>
-      </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A232" s="2">
         <v>413</v>
       </c>
@@ -8646,11 +7949,8 @@
       <c r="H232">
         <v>8.09</v>
       </c>
-      <c r="I232">
-        <v>194.16</v>
-      </c>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A233" s="2">
         <v>415</v>
       </c>
@@ -8675,11 +7975,8 @@
       <c r="H233">
         <v>8.09</v>
       </c>
-      <c r="I233">
-        <v>194.16</v>
-      </c>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A234" s="2">
         <v>422</v>
       </c>
@@ -8704,11 +8001,8 @@
       <c r="H234">
         <v>6.29</v>
       </c>
-      <c r="I234">
-        <v>75.48</v>
-      </c>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>423</v>
       </c>
@@ -8733,11 +8027,8 @@
       <c r="H235" s="4">
         <v>6.29</v>
       </c>
-      <c r="I235" s="4">
-        <v>75.48</v>
-      </c>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A236" s="2">
         <v>424</v>
       </c>
@@ -8762,11 +8053,8 @@
       <c r="H236">
         <v>6.29</v>
       </c>
-      <c r="I236">
-        <v>75.48</v>
-      </c>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A237" s="2">
         <v>430</v>
       </c>
@@ -8791,11 +8079,8 @@
       <c r="H237">
         <v>8.09</v>
       </c>
-      <c r="I237">
-        <v>194.16</v>
-      </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A238" s="2">
         <v>433</v>
       </c>
@@ -8820,11 +8105,8 @@
       <c r="H238">
         <v>6.29</v>
       </c>
-      <c r="I238">
-        <v>75.48</v>
-      </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="2">
         <v>435</v>
       </c>
@@ -8849,11 +8131,8 @@
       <c r="H239">
         <v>6.29</v>
       </c>
-      <c r="I239">
-        <v>75.48</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="2">
         <v>442</v>
       </c>
@@ -8878,11 +8157,8 @@
       <c r="H240">
         <v>6.29</v>
       </c>
-      <c r="I240">
-        <v>75.48</v>
-      </c>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="2">
         <v>456</v>
       </c>
@@ -8907,11 +8183,8 @@
       <c r="H241">
         <v>6.29</v>
       </c>
-      <c r="I241">
-        <v>150.96</v>
-      </c>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="2">
         <v>467</v>
       </c>
@@ -8935,9 +8208,6 @@
       </c>
       <c r="H242">
         <v>6.29</v>
-      </c>
-      <c r="I242">
-        <v>75.48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>